<commit_message>
finished legendre model equation.  Commit before finishing on work computer
</commit_message>
<xml_diff>
--- a/MeiTreeOutput.xlsx
+++ b/MeiTreeOutput.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="27795" windowHeight="13350" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="order2" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
   <si>
     <t>Coefficient</t>
   </si>
@@ -36,94 +36,40 @@
     <t>(Intercept)</t>
   </si>
   <si>
-    <t xml:space="preserve">0.0174 *  </t>
-  </si>
-  <si>
     <t xml:space="preserve">AATTC_nn_np_2517_a                     </t>
   </si>
   <si>
-    <t>5.13e-09 ***</t>
-  </si>
-  <si>
     <t xml:space="preserve">AATTC_nn_np_2815_a                     </t>
   </si>
   <si>
-    <t xml:space="preserve">0.0221 *  </t>
-  </si>
-  <si>
     <t xml:space="preserve">CATG_nn_np_3479_a                      </t>
   </si>
   <si>
-    <t>1.63e-05 ***</t>
-  </si>
-  <si>
     <t xml:space="preserve">CATG_nn_np_1284_a                      </t>
   </si>
   <si>
-    <t>4.61e-05 ***</t>
-  </si>
-  <si>
     <t xml:space="preserve">AATTC_nn_np_2815_a×AATTC_lm_ll_3034_a  </t>
   </si>
   <si>
-    <t>1.71e-06 ***</t>
-  </si>
-  <si>
-    <t>0.00415 **</t>
-  </si>
-  <si>
-    <t>2.27e-09 ***</t>
-  </si>
-  <si>
-    <t>1.54e-06 ***</t>
-  </si>
-  <si>
-    <t>1.23e-08 ***</t>
-  </si>
-  <si>
-    <t>&lt; 2e-16 ***</t>
-  </si>
-  <si>
     <t xml:space="preserve">AATTC_nn_np_2815_a×AATTC_hk_hk_278_a                      </t>
   </si>
   <si>
-    <t>3.48e-10 ***</t>
-  </si>
-  <si>
     <t xml:space="preserve">CATG_lm_ll_3153_a                                         </t>
   </si>
   <si>
-    <t>3.36e-05 ***</t>
-  </si>
-  <si>
     <t xml:space="preserve">CATG_nn_np_1284_a×AATTC_nn_np_554_a                       </t>
   </si>
   <si>
-    <t>1.23e-05 ***</t>
-  </si>
-  <si>
     <t>AATTC_nn_np_2815_a.AATTC_lm_ll_3034_a×AATTC_nn_np_1615_a</t>
   </si>
   <si>
-    <t>2.39e-13 ***</t>
-  </si>
-  <si>
     <t xml:space="preserve">AATTC_nn_np_2815_a×AATTC_nn_np_929_a                     </t>
   </si>
   <si>
-    <t>7.57e-08 ***</t>
-  </si>
-  <si>
     <t xml:space="preserve">AATTC_hk_hk_479_d                                         </t>
   </si>
   <si>
-    <t>6.37e-06 ***</t>
-  </si>
-  <si>
     <t xml:space="preserve">AATTC_nn_np_2517_a×CATG_hk_hk_648_a                       </t>
-  </si>
-  <si>
-    <t>8.33e-07 ***</t>
   </si>
   <si>
     <t>mu_t</t>
@@ -199,6 +145,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -228,8 +177,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,8 +483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,13 +519,13 @@
       <c r="D2">
         <v>2.4020000000000001</v>
       </c>
-      <c r="E2" t="s">
-        <v>6</v>
+      <c r="E2" s="1">
+        <v>1.7399999999999999E-2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>0.40012999999999999</v>
@@ -586,13 +536,13 @@
       <c r="D3">
         <v>6.1470000000000002</v>
       </c>
-      <c r="E3" t="s">
-        <v>8</v>
+      <c r="E3" s="1">
+        <v>5.1300000000000003E-9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>0.15792</v>
@@ -603,13 +553,13 @@
       <c r="D4">
         <v>2.31</v>
       </c>
-      <c r="E4" t="s">
-        <v>10</v>
+      <c r="E4" s="1">
+        <v>2.2100000000000002E-2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>0.23433000000000001</v>
@@ -620,13 +570,13 @@
       <c r="D5">
         <v>4.4340000000000002</v>
       </c>
-      <c r="E5" t="s">
-        <v>12</v>
+      <c r="E5" s="1">
+        <v>1.63E-5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>0.222</v>
@@ -637,13 +587,13 @@
       <c r="D6">
         <v>4.1790000000000003</v>
       </c>
-      <c r="E6" t="s">
-        <v>14</v>
+      <c r="E6" s="1">
+        <v>4.6100000000000002E-5</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>0.45783000000000001</v>
@@ -654,8 +604,8 @@
       <c r="D7">
         <v>4.9530000000000003</v>
       </c>
-      <c r="E7" t="s">
-        <v>16</v>
+      <c r="E7" s="1">
+        <v>1.7099999999999999E-6</v>
       </c>
     </row>
   </sheetData>
@@ -668,10 +618,14 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="61" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -703,13 +657,13 @@
       <c r="D2">
         <v>2.9060000000000001</v>
       </c>
-      <c r="E2" t="s">
-        <v>17</v>
+      <c r="E2" s="1">
+        <v>4.15E-3</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>0.27772999999999998</v>
@@ -720,13 +674,13 @@
       <c r="D3">
         <v>6.3179999999999996</v>
       </c>
-      <c r="E3" t="s">
-        <v>18</v>
+      <c r="E3" s="1">
+        <v>2.2699999999999998E-9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>0.26382</v>
@@ -737,13 +691,13 @@
       <c r="D4">
         <v>4.9829999999999997</v>
       </c>
-      <c r="E4" t="s">
-        <v>19</v>
+      <c r="E4" s="1">
+        <v>1.5400000000000001E-6</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>0.20766999999999999</v>
@@ -754,13 +708,13 @@
       <c r="D5">
         <v>5.99</v>
       </c>
-      <c r="E5" t="s">
-        <v>20</v>
+      <c r="E5" s="1">
+        <v>1.2299999999999999E-8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>4.5220000000000003E-2</v>
@@ -771,13 +725,13 @@
       <c r="D6">
         <v>1.06</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>0.29054999999999997</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>1.82572</v>
@@ -788,13 +742,13 @@
       <c r="D7">
         <v>10.185</v>
       </c>
-      <c r="E7" t="s">
-        <v>21</v>
+      <c r="E7" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>0.25935000000000002</v>
@@ -805,13 +759,13 @@
       <c r="D8">
         <v>6.6710000000000003</v>
       </c>
-      <c r="E8" t="s">
-        <v>23</v>
+      <c r="E8" s="1">
+        <v>3.4799999999999999E-10</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <v>0.14877000000000001</v>
@@ -822,13 +776,13 @@
       <c r="D9">
         <v>4.2619999999999996</v>
       </c>
-      <c r="E9" t="s">
-        <v>25</v>
+      <c r="E9" s="1">
+        <v>3.3599999999999997E-5</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="B10">
         <v>0.22994000000000001</v>
@@ -839,13 +793,13 @@
       <c r="D10">
         <v>4.5049999999999999</v>
       </c>
-      <c r="E10" t="s">
-        <v>27</v>
+      <c r="E10" s="1">
+        <v>1.2300000000000001E-5</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>-1.5171399999999999</v>
@@ -856,13 +810,13 @@
       <c r="D11">
         <v>-7.96</v>
       </c>
-      <c r="E11" t="s">
-        <v>29</v>
+      <c r="E11" s="1">
+        <v>2.3899999999999999E-13</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="B12">
         <v>-0.30804999999999999</v>
@@ -873,13 +827,13 @@
       <c r="D12">
         <v>-5.6239999999999997</v>
       </c>
-      <c r="E12" t="s">
-        <v>31</v>
+      <c r="E12" s="1">
+        <v>7.5699999999999996E-8</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="B13">
         <v>0.16044</v>
@@ -890,13 +844,13 @@
       <c r="D13">
         <v>4.66</v>
       </c>
-      <c r="E13" t="s">
-        <v>33</v>
+      <c r="E13" s="1">
+        <v>6.37E-6</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>0.14537</v>
@@ -907,8 +861,8 @@
       <c r="D14">
         <v>5.1180000000000003</v>
       </c>
-      <c r="E14" t="s">
-        <v>35</v>
+      <c r="E14" s="1">
+        <v>8.3300000000000001E-7</v>
       </c>
     </row>
   </sheetData>
@@ -920,8 +874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F19:F20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="A1:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -945,7 +899,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="B2">
         <v>0.98465000000000003</v>
@@ -962,7 +916,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="B3">
         <v>-18.346029999999999</v>
@@ -979,7 +933,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="B4">
         <v>15.099780000000001</v>
@@ -996,7 +950,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="B5">
         <v>17.447340000000001</v>
@@ -1013,7 +967,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="B6">
         <v>35.646279999999997</v>
@@ -1030,7 +984,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="B7">
         <v>-20.863209999999999</v>
@@ -1047,7 +1001,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="B8">
         <v>11.635120000000001</v>
@@ -1064,7 +1018,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="B9">
         <v>-22.107399999999998</v>
@@ -1081,7 +1035,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="B10">
         <v>-16.8444</v>
@@ -1098,7 +1052,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="B11">
         <v>-13.80524</v>
@@ -1115,7 +1069,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="B12">
         <v>18.90166</v>
@@ -1132,7 +1086,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="B13">
         <v>-7.2606999999999999</v>
@@ -1149,7 +1103,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="B14">
         <v>7.81921</v>
@@ -1166,7 +1120,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="B15">
         <v>-15.91187</v>
@@ -1183,7 +1137,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="B16">
         <v>-13.769590000000001</v>
@@ -1200,7 +1154,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="B17">
         <v>-8.9870400000000004</v>
@@ -1217,7 +1171,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="B18">
         <v>23.976520000000001</v>
@@ -1234,7 +1188,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="B19">
         <v>-18.612590000000001</v>
@@ -1251,7 +1205,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="B20">
         <v>-11.7958</v>
@@ -1268,7 +1222,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="B21">
         <v>8.1659299999999995</v>
@@ -1285,7 +1239,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="B22">
         <v>9.5687300000000004</v>
@@ -1302,7 +1256,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="B23">
         <v>-8.6498299999999997</v>
@@ -1319,7 +1273,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="B24">
         <v>14.27351</v>

</xml_diff>